<commit_message>
Excel Table X update
</commit_message>
<xml_diff>
--- a/Table X - SurfaceVariables/Table-X-SurfaceVariables.xlsx
+++ b/Table X - SurfaceVariables/Table-X-SurfaceVariables.xlsx
@@ -404,7 +404,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -432,6 +432,10 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1144,7 +1148,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="H23" sqref="H23:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1497,7 +1501,9 @@
       <c r="C23" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="6"/>
+      <c r="D23" s="13">
+        <v>14.9964190582785</v>
+      </c>
       <c r="E23" s="11" t="s">
         <v>64</v>
       </c>
@@ -1506,6 +1512,9 @@
       </c>
       <c r="G23" s="6" t="s">
         <v>37</v>
+      </c>
+      <c r="H23" s="14">
+        <v>16.921301270796899</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1518,7 +1527,9 @@
       <c r="C24" s="7">
         <v>39893</v>
       </c>
-      <c r="D24" s="7"/>
+      <c r="D24" s="13">
+        <v>14.481906897791999</v>
+      </c>
       <c r="E24" s="11" t="s">
         <v>65</v>
       </c>
@@ -1527,6 +1538,9 @@
       </c>
       <c r="G24" s="8" t="s">
         <v>40</v>
+      </c>
+      <c r="H24" s="14">
+        <v>14.734212145307801</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1539,7 +1553,9 @@
       <c r="C25" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="8"/>
+      <c r="D25" s="13">
+        <v>14.2431107560074</v>
+      </c>
       <c r="E25" s="10" t="s">
         <v>66</v>
       </c>
@@ -1548,6 +1564,9 @@
       </c>
       <c r="G25" s="6" t="s">
         <v>41</v>
+      </c>
+      <c r="H25" s="14">
+        <v>14.5142202430478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>